<commit_message>
Updated templates and application
</commit_message>
<xml_diff>
--- a/ProjectMaker/.templates/Project_vii_TEMPLATE/Project_assessment_vii.xlsx
+++ b/ProjectMaker/.templates/Project_vii_TEMPLATE/Project_assessment_vii.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
   </bookViews>
   <sheets>
     <sheet name="costs (SI metric)" sheetId="6" r:id="rId1"/>
@@ -261,9 +261,6 @@
     <t>rootwad</t>
   </si>
   <si>
-    <t>Engineered log jam: complete</t>
-  </si>
-  <si>
     <t>Cramer (2012)
 Knutson (2015)</t>
   </si>
@@ -574,11 +571,14 @@
     <t>Terrain stabilization</t>
   </si>
   <si>
-    <t>Streamwood
+    <t>Anchoring (logs for plant stability)</t>
+  </si>
+  <si>
+    <t>Engineered log jam, log-wise
 (for plant and terrain stabilization)</t>
   </si>
   <si>
-    <t>Anchoring (logs for plant stability)</t>
+    <t>Streamwood (non-anchored)</t>
   </si>
 </sst>
 </file>
@@ -1988,8 +1988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2010,7 +2010,7 @@
   <sheetData>
     <row r="1" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="186" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" s="186"/>
       <c r="D1" s="186"/>
@@ -2033,7 +2033,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="187" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I2" s="188" t="str">
         <f>IF(NOT(OR(ISBLANK(G2), ISBLANK(G3))),G2/G3,"")</f>
@@ -2041,7 +2041,7 @@
       </c>
       <c r="J2" s="81"/>
       <c r="K2" s="189" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2049,11 +2049,11 @@
         <v>1</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="80"/>
       <c r="E3" s="191" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F3" s="172"/>
       <c r="G3" s="99"/>
@@ -2119,7 +2119,7 @@
         <v>5.4399999999999997E-2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="127">
         <f>from_geodata!C8</f>
@@ -2143,7 +2143,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F8" s="57" t="s">
         <v>16</v>
@@ -2156,7 +2156,7 @@
         <v>17</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="2:11" s="140" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2207,16 +2207,16 @@
     </row>
     <row r="12" spans="2:11" s="140" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="183" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D12" s="132">
         <v>80</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F12" s="127">
         <f>(from_geodata!C13)/log_length</f>
@@ -2246,7 +2246,7 @@
         <v>24</v>
       </c>
       <c r="F13" s="126">
-        <f>(from_geodata!C12  + from_geodata!C13+ from_geodata!F12)/log_length^2</f>
+        <f>( from_geodata!C13)/square_yd2acre/ft2yd^2/log_length^2</f>
         <v>0</v>
       </c>
       <c r="G13" s="152">
@@ -2279,44 +2279,47 @@
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="2:11" s="145" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="167"/>
       <c r="C15" s="5" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="D15" s="135">
-        <f>AVERAGE(5000,20000, 30000, 100000)</f>
-        <v>38750</v>
+        <f>AVERAGE(600,1000, 300, 1200)</f>
+        <v>775</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="52"/>
+      <c r="F15" s="126">
+        <f>(from_geodata!C12 + from_geodata!F12)/square_yd2acre/ft2yd^2/log_length^2</f>
+        <v>0</v>
+      </c>
       <c r="G15" s="152">
         <f>F15*D15</f>
         <v>0</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:11" s="145" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="167"/>
       <c r="C16" s="64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="136">
         <v>150</v>
       </c>
       <c r="E16" s="65" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F16" s="126">
-        <f>(from_geodata!C16 + from_geodata!F15)</f>
+        <f>(from_geodata!C16 + from_geodata!C15)/ square_yd2acre</f>
         <v>0</v>
       </c>
       <c r="G16" s="156">
@@ -2325,12 +2328,12 @@
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:9" s="145" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="181" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" s="167"/>
       <c r="D17" s="167"/>
@@ -2355,10 +2358,10 @@
     </row>
     <row r="19" spans="2:9" s="145" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="183" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="D19" s="133">
         <f>AVERAGE(120, 300)</f>
@@ -2374,20 +2377,20 @@
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="169"/>
       <c r="C20" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="137">
         <f>20*1.65</f>
         <v>33</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" s="53"/>
       <c r="G20" s="157">
@@ -2396,19 +2399,19 @@
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="2:9" s="145" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="167"/>
       <c r="C21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="133">
         <v>18</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F21" s="52"/>
       <c r="G21" s="152">
@@ -2416,22 +2419,22 @@
         <v>0</v>
       </c>
       <c r="H21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:9" s="145" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="167"/>
       <c r="C22" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="133">
         <v>18</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F22" s="52"/>
       <c r="G22" s="152">
@@ -2439,22 +2442,22 @@
         <v>0</v>
       </c>
       <c r="H22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:9" s="145" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="167"/>
       <c r="C23" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="133">
         <v>10</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F23" s="126">
         <f>from_geodata!C5</f>
@@ -2465,22 +2468,22 @@
         <v>0</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="2:9" s="145" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="167"/>
       <c r="C24" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="133">
         <v>10</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F24" s="126">
         <f>from_geodata!C7</f>
@@ -2491,22 +2494,22 @@
         <v>0</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="169"/>
       <c r="C25" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="138">
         <v>10</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F25" s="128">
         <f>from_geodata!C4</f>
@@ -2518,19 +2521,19 @@
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="169"/>
       <c r="C26" s="67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" s="139">
         <v>10</v>
       </c>
       <c r="E26" s="68" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F26" s="128">
         <f>from_geodata!C6</f>
@@ -2542,12 +2545,12 @@
       </c>
       <c r="H26" s="24"/>
       <c r="I26" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="181" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="169"/>
       <c r="D27" s="170"/>
@@ -2572,16 +2575,16 @@
     </row>
     <row r="29" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="184" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="D29" s="137">
         <v>75</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F29" s="53"/>
       <c r="G29" s="157">
@@ -2589,7 +2592,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I29" s="12" t="s">
         <v>20</v>
@@ -2598,13 +2601,13 @@
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="169"/>
       <c r="C30" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" s="137">
         <v>35</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F30" s="53"/>
       <c r="G30" s="157">
@@ -2612,7 +2615,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>20</v>
@@ -2621,14 +2624,14 @@
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="169"/>
       <c r="C31" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" s="137">
         <f>(2+10)/2</f>
         <v>6</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F31" s="53"/>
       <c r="G31" s="157">
@@ -2636,7 +2639,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>20</v>
@@ -2645,14 +2648,14 @@
     <row r="32" spans="2:9" s="145" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="167"/>
       <c r="C32" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D32" s="133">
         <f>(10+20)/2</f>
         <v>15</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F32" s="126">
         <f>(from_geodata!C14 + from_geodata!F13)</f>
@@ -2663,7 +2666,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>20</v>
@@ -2672,17 +2675,17 @@
     <row r="33" spans="2:9" s="145" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="167"/>
       <c r="C33" s="64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D33" s="136">
         <f>(120+160)/2</f>
         <v>140</v>
       </c>
       <c r="E33" s="65" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F33" s="126">
-        <f>(from_geodata!C15 + from_geodata!F14)</f>
+        <f>(from_geodata!F15 + from_geodata!F14)</f>
         <v>0</v>
       </c>
       <c r="G33" s="156">
@@ -2690,7 +2693,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I33" s="18" t="s">
         <v>20</v>
@@ -2698,7 +2701,7 @@
     </row>
     <row r="34" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="181" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="169"/>
       <c r="D34" s="170"/>
@@ -2723,16 +2726,16 @@
     </row>
     <row r="36" spans="2:9" s="145" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="183" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="D36" s="133">
         <v>0.93</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F36" s="52"/>
       <c r="G36" s="152">
@@ -2741,20 +2744,20 @@
       </c>
       <c r="H36" s="7"/>
       <c r="I36" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="2:9" s="145" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="167"/>
       <c r="C37" s="64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D37" s="136">
         <f>AVERAGE(1000, 2000)</f>
         <v>1500</v>
       </c>
       <c r="E37" s="65" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F37" s="66"/>
       <c r="G37" s="156">
@@ -2763,12 +2766,12 @@
       </c>
       <c r="H37" s="17"/>
       <c r="I37" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="2:9" s="145" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="181" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C38" s="167"/>
       <c r="D38" s="167"/>
@@ -2793,16 +2796,16 @@
     </row>
     <row r="40" spans="2:9" s="145" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="183" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="D40" s="133">
         <v>200</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F40" s="52"/>
       <c r="G40" s="152">
@@ -2817,13 +2820,13 @@
     <row r="41" spans="2:9" s="145" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="167"/>
       <c r="C41" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D41" s="133">
         <v>1500</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F41" s="52"/>
       <c r="G41" s="152">
@@ -2838,13 +2841,13 @@
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="169"/>
       <c r="C42" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D42" s="137">
         <v>100</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F42" s="53"/>
       <c r="G42" s="157">
@@ -2852,7 +2855,7 @@
         <v>0</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I42" s="12" t="s">
         <v>13</v>
@@ -2861,13 +2864,13 @@
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="169"/>
       <c r="C43" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D43" s="137">
         <v>140</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F43" s="53"/>
       <c r="G43" s="157">
@@ -2882,13 +2885,13 @@
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="169"/>
       <c r="C44" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D44" s="137">
         <v>275</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F44" s="53"/>
       <c r="G44" s="157">
@@ -2903,13 +2906,13 @@
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="169"/>
       <c r="C45" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D45" s="137">
         <v>850</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F45" s="53"/>
       <c r="G45" s="157">
@@ -2924,13 +2927,13 @@
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" s="169"/>
       <c r="C46" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D46" s="137">
         <v>1250</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F46" s="53"/>
       <c r="G46" s="157">
@@ -2945,14 +2948,14 @@
     <row r="47" spans="2:9" s="145" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="167"/>
       <c r="C47" s="64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D47" s="136">
         <f>AVERAGE(3.29, 4.21, 5.65, 2.57, 2.77)*0.91^2</f>
         <v>3.0623138000000005</v>
       </c>
       <c r="E47" s="65" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F47" s="66"/>
       <c r="G47" s="156">
@@ -2961,12 +2964,12 @@
       </c>
       <c r="H47" s="17"/>
       <c r="I47" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="2:9" s="145" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="181" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C48" s="167"/>
       <c r="D48" s="167"/>
@@ -2991,7 +2994,7 @@
     </row>
     <row r="50" spans="2:9" s="145" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="180" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C50" s="167"/>
       <c r="D50" s="167"/>
@@ -3006,7 +3009,7 @@
     </row>
     <row r="52" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="173" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C52" s="169"/>
       <c r="D52" s="170"/>
@@ -3028,7 +3031,7 @@
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" s="177" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C54" s="169"/>
       <c r="D54" s="31"/>
@@ -3040,14 +3043,14 @@
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" s="178" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C55" s="169"/>
       <c r="D55" s="34">
         <v>0.1</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F55" s="143">
         <v>1</v>
@@ -3062,14 +3065,14 @@
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" s="178" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C56" s="169"/>
       <c r="D56" s="35">
         <v>0.1</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F56" s="143">
         <v>1</v>
@@ -3084,7 +3087,7 @@
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" s="177" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C57" s="169"/>
       <c r="D57" s="36"/>
@@ -3096,14 +3099,14 @@
     </row>
     <row r="58" spans="2:9" s="145" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="179" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C58" s="167"/>
       <c r="D58" s="131">
         <v>0.16500000000000001</v>
       </c>
       <c r="E58" s="59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F58" s="60">
         <v>1</v>
@@ -3114,19 +3117,19 @@
       </c>
       <c r="H58" s="37"/>
       <c r="I58" s="38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="2:9" s="145" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="166" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C59" s="167"/>
       <c r="D59" s="58">
         <v>0.35</v>
       </c>
       <c r="E59" s="59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F59" s="60">
         <v>1</v>
@@ -3143,7 +3146,7 @@
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" s="168" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C61" s="169"/>
       <c r="D61" s="170"/>
@@ -3216,8 +3219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3238,7 +3241,7 @@
   <sheetData>
     <row r="1" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="186" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C1" s="186"/>
       <c r="D1" s="186"/>
@@ -3261,7 +3264,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="187" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I2" s="188" t="str">
         <f>IF(NOT(OR(ISBLANK(G2), ISBLANK(G3))),G2/G3,"")</f>
@@ -3269,7 +3272,7 @@
       </c>
       <c r="J2" s="81"/>
       <c r="K2" s="189" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3277,11 +3280,11 @@
         <v>1</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="80"/>
       <c r="E3" s="191" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F3" s="172"/>
       <c r="G3" s="99"/>
@@ -3384,7 +3387,7 @@
         <v>17</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="2:11" s="91" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3435,10 +3438,10 @@
     </row>
     <row r="12" spans="2:11" s="91" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="183" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D12" s="105">
         <v>80</v>
@@ -3474,7 +3477,7 @@
         <v>24</v>
       </c>
       <c r="F13" s="126">
-        <f>(from_geodata!C12  + from_geodata!C13+ from_geodata!F12)/square_yd2acre/ft2yd^2/log_length^2</f>
+        <f>( from_geodata!C13)/square_yd2acre/ft2yd^2/log_length^2</f>
         <v>0</v>
       </c>
       <c r="G13" s="108">
@@ -3507,44 +3510,47 @@
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="2:11" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="167"/>
       <c r="C15" s="5" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="D15" s="113">
-        <f>AVERAGE(5000,20000, 30000, 100000)</f>
-        <v>38750</v>
+        <f>AVERAGE(600,1000, 300, 1200)</f>
+        <v>775</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="52"/>
+        <v>24</v>
+      </c>
+      <c r="F15" s="126">
+        <f>(from_geodata!C12 + from_geodata!F12)/square_yd2acre/ft2yd^2/log_length^2</f>
+        <v>0</v>
+      </c>
       <c r="G15" s="108">
         <f>F15*D15</f>
         <v>0</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:11" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="167"/>
       <c r="C16" s="64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="114">
         <v>150</v>
       </c>
       <c r="E16" s="65" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="126">
-        <f>(from_geodata!C16 + from_geodata!F15)/ square_yd2acre</f>
+        <f>(from_geodata!C16 + from_geodata!C15)/ square_yd2acre</f>
         <v>0</v>
       </c>
       <c r="G16" s="115">
@@ -3553,12 +3559,12 @@
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="181" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" s="167"/>
       <c r="D17" s="167"/>
@@ -3583,10 +3589,10 @@
     </row>
     <row r="19" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="183" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="D19" s="107">
         <f>AVERAGE(120, 300)</f>
@@ -3602,20 +3608,20 @@
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="169"/>
       <c r="C20" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="116">
         <f>20*1.65</f>
         <v>33</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" s="53"/>
       <c r="G20" s="117">
@@ -3624,13 +3630,13 @@
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="167"/>
       <c r="C21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="107">
         <f>AVERAGE(73059, 71836)</f>
@@ -3645,16 +3651,16 @@
         <v>0</v>
       </c>
       <c r="H21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="167"/>
       <c r="C22" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="107">
         <f>AVERAGE(73059, 71836)</f>
@@ -3669,16 +3675,16 @@
         <v>0</v>
       </c>
       <c r="H22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="167"/>
       <c r="C23" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="107">
         <v>40598</v>
@@ -3695,16 +3701,16 @@
         <v>0</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="167"/>
       <c r="C24" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="107">
         <v>40598</v>
@@ -3721,16 +3727,16 @@
         <v>0</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="169"/>
       <c r="C25" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="118">
         <f>AVERAGE(35000,45000)</f>
@@ -3749,13 +3755,13 @@
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="169"/>
       <c r="C26" s="67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" s="119">
         <f>AVERAGE(35000,45000)</f>
@@ -3774,12 +3780,12 @@
       </c>
       <c r="H26" s="24"/>
       <c r="I26" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="181" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="169"/>
       <c r="D27" s="170"/>
@@ -3804,17 +3810,17 @@
     </row>
     <row r="29" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="184" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="D29" s="116">
         <f>(60+100)/2</f>
         <v>80</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F29" s="53"/>
       <c r="G29" s="117">
@@ -3822,7 +3828,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I29" s="12" t="s">
         <v>20</v>
@@ -3831,7 +3837,7 @@
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="169"/>
       <c r="C30" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" s="116">
         <f>(25+50)/2</f>
@@ -3846,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>20</v>
@@ -3855,14 +3861,14 @@
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="169"/>
       <c r="C31" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" s="116">
         <f>(3+12)/2</f>
         <v>7.5</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F31" s="53"/>
       <c r="G31" s="117">
@@ -3870,7 +3876,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I31" s="12" t="s">
         <v>20</v>
@@ -3879,7 +3885,7 @@
     <row r="32" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="167"/>
       <c r="C32" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D32" s="107">
         <f>(10+20)/2</f>
@@ -3897,7 +3903,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>20</v>
@@ -3906,17 +3912,17 @@
     <row r="33" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="167"/>
       <c r="C33" s="64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D33" s="114">
         <f>(140+175)/2</f>
         <v>157.5</v>
       </c>
       <c r="E33" s="65" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F33" s="126">
-        <f>(from_geodata!C15 + from_geodata!F14)*square_yd2acre</f>
+        <f>(from_geodata!F15 + from_geodata!F14)</f>
         <v>0</v>
       </c>
       <c r="G33" s="115">
@@ -3924,7 +3930,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I33" s="18" t="s">
         <v>20</v>
@@ -3932,7 +3938,7 @@
     </row>
     <row r="34" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="181" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="169"/>
       <c r="D34" s="170"/>
@@ -3957,10 +3963,10 @@
     </row>
     <row r="36" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="183" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="D36" s="107">
         <f>AVERAGE(2500, 5000)</f>
@@ -3976,13 +3982,13 @@
       </c>
       <c r="H36" s="7"/>
       <c r="I36" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="167"/>
       <c r="C37" s="64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D37" s="114">
         <f>AVERAGE(1000, 2000)</f>
@@ -3998,12 +4004,12 @@
       </c>
       <c r="H37" s="17"/>
       <c r="I37" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="181" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C38" s="167"/>
       <c r="D38" s="167"/>
@@ -4028,10 +4034,10 @@
     </row>
     <row r="40" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="183" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="D40" s="107">
         <v>250</v>
@@ -4052,14 +4058,14 @@
     <row r="41" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="167"/>
       <c r="C41" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D41" s="107">
         <f>1700*0.9071847</f>
         <v>1542.21399</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F41" s="52"/>
       <c r="G41" s="108">
@@ -4074,7 +4080,7 @@
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="169"/>
       <c r="C42" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D42" s="116">
         <v>100</v>
@@ -4095,7 +4101,7 @@
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="169"/>
       <c r="C43" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D43" s="116">
         <v>150</v>
@@ -4116,7 +4122,7 @@
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="169"/>
       <c r="C44" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D44" s="116">
         <v>300</v>
@@ -4137,13 +4143,13 @@
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="169"/>
       <c r="C45" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D45" s="116">
         <v>1000</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F45" s="53"/>
       <c r="G45" s="117">
@@ -4158,13 +4164,13 @@
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" s="169"/>
       <c r="C46" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D46" s="116">
         <v>1500</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F46" s="53"/>
       <c r="G46" s="117">
@@ -4179,14 +4185,14 @@
     <row r="47" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="167"/>
       <c r="C47" s="64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D47" s="114">
         <f>AVERAGE(3.29, 4.21, 5.65, 2.57, 2.77)</f>
         <v>3.6980000000000004</v>
       </c>
       <c r="E47" s="65" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F47" s="66"/>
       <c r="G47" s="115">
@@ -4195,12 +4201,12 @@
       </c>
       <c r="H47" s="17"/>
       <c r="I47" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="181" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C48" s="167"/>
       <c r="D48" s="167"/>
@@ -4225,7 +4231,7 @@
     </row>
     <row r="50" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="180" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C50" s="167"/>
       <c r="D50" s="167"/>
@@ -4240,7 +4246,7 @@
     </row>
     <row r="52" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="173" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C52" s="169"/>
       <c r="D52" s="170"/>
@@ -4262,7 +4268,7 @@
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" s="177" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C54" s="169"/>
       <c r="D54" s="31"/>
@@ -4274,14 +4280,14 @@
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" s="178" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C55" s="169"/>
       <c r="D55" s="34">
         <v>0.1</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F55" s="85">
         <v>1</v>
@@ -4296,14 +4302,14 @@
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" s="178" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C56" s="169"/>
       <c r="D56" s="35">
         <v>0.1</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F56" s="85">
         <v>1</v>
@@ -4318,7 +4324,7 @@
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" s="177" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C57" s="169"/>
       <c r="D57" s="36"/>
@@ -4330,14 +4336,14 @@
     </row>
     <row r="58" spans="2:9" s="90" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="179" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C58" s="167"/>
       <c r="D58" s="131">
         <v>0.16500000000000001</v>
       </c>
       <c r="E58" s="59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F58" s="60">
         <v>1</v>
@@ -4348,19 +4354,19 @@
       </c>
       <c r="H58" s="37"/>
       <c r="I58" s="38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="166" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C59" s="167"/>
       <c r="D59" s="58">
         <v>0.35</v>
       </c>
       <c r="E59" s="59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F59" s="60">
         <v>1</v>
@@ -4374,7 +4380,7 @@
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" s="168" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C61" s="169"/>
       <c r="D61" s="170"/>
@@ -4448,7 +4454,7 @@
   <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4465,37 +4471,37 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="94" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="94" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="94" t="s">
         <v>87</v>
-      </c>
-      <c r="C3" s="94" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="94" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10" s="94" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="94" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="94" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="94" t="s">
-        <v>88</v>
-      </c>
       <c r="E11" s="94" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="94" t="s">
         <v>87</v>
-      </c>
-      <c r="F11" s="94" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -4525,10 +4531,10 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="94" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" s="192" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D2" s="193"/>
       <c r="E2" s="193"/>
@@ -4539,7 +4545,7 @@
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="194" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" s="195"/>
       <c r="D3" s="195"/>
@@ -4561,20 +4567,20 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="94" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="56"/>
       <c r="D5" s="94" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="56"/>
       <c r="D6" s="94" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>